<commit_message>
fix bug about select operation group
</commit_message>
<xml_diff>
--- a/Docs/06 Testing/测试课题.xlsx
+++ b/Docs/06 Testing/测试课题.xlsx
@@ -3236,7 +3236,7 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1142408</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>621712</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3280,7 +3280,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>3743</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>590893</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3324,7 +3324,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1148857</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>462328</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3715,7 +3715,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1226530</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>495300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3758,7 +3758,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2243</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>694765</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3883,7 +3883,7 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1101588</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>504253</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3927,7 +3927,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>3479</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>595841</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4123,7 +4123,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2698</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>502227</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4167,7 +4167,7 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1038225</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>520476</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4289,7 +4289,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>588994</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4333,7 +4333,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1133914</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>542268</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4376,7 +4376,7 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1141239</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>621712</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4420,7 +4420,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>916</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>590893</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7076,8 +7076,8 @@
   <dimension ref="A1:Q232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M54" sqref="M54"/>
+      <pane ySplit="3" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -8966,7 +8966,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="53" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A53" s="152">
         <v>50</v>
       </c>
@@ -9001,7 +9001,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:17" s="17" customFormat="1" ht="75.599999999999994" customHeight="1">
+    <row r="54" spans="1:17" s="17" customFormat="1" ht="75.599999999999994" hidden="1" customHeight="1">
       <c r="A54" s="152">
         <v>51</v>
       </c>
@@ -9034,7 +9034,7 @@
       </c>
       <c r="Q54" s="220"/>
     </row>
-    <row r="55" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="55" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A55" s="152">
         <v>52</v>
       </c>
@@ -9069,7 +9069,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="56" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="56" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A56" s="152">
         <v>53</v>
       </c>
@@ -9100,7 +9100,7 @@
       <c r="P56" s="211"/>
       <c r="Q56" s="220"/>
     </row>
-    <row r="57" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="57" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A57" s="152">
         <v>54</v>
       </c>
@@ -9131,7 +9131,7 @@
       <c r="P57" s="211"/>
       <c r="Q57" s="220"/>
     </row>
-    <row r="58" spans="1:17" s="17" customFormat="1" ht="100.8">
+    <row r="58" spans="1:17" s="17" customFormat="1" ht="100.8" hidden="1">
       <c r="A58" s="152">
         <v>55</v>
       </c>
@@ -9191,7 +9191,7 @@
       <c r="P59" s="211"/>
       <c r="Q59" s="220"/>
     </row>
-    <row r="60" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="60" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A60" s="152">
         <v>57</v>
       </c>
@@ -9471,7 +9471,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="70" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="70" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A70" s="152">
         <v>67</v>
       </c>
@@ -9887,7 +9887,7 @@
       </c>
       <c r="Q83" s="235"/>
     </row>
-    <row r="84" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="84" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A84" s="152">
         <v>81</v>
       </c>
@@ -10005,7 +10005,7 @@
       <c r="P87" s="150"/>
       <c r="Q87" s="151"/>
     </row>
-    <row r="88" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="88" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A88" s="152">
         <v>85</v>
       </c>
@@ -10096,7 +10096,7 @@
       <c r="P90" s="150"/>
       <c r="Q90" s="151"/>
     </row>
-    <row r="91" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="91" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A91" s="152">
         <v>88</v>
       </c>
@@ -10444,7 +10444,7 @@
       <c r="P102" s="150"/>
       <c r="Q102" s="151"/>
     </row>
-    <row r="103" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="103" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A103" s="152">
         <v>100</v>
       </c>
@@ -10568,7 +10568,7 @@
       <c r="P106" s="211"/>
       <c r="Q106" s="220"/>
     </row>
-    <row r="107" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="107" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A107" s="152">
         <v>104</v>
       </c>
@@ -10657,7 +10657,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="110" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="110" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A110" s="152">
         <v>107</v>
       </c>
@@ -10686,7 +10686,7 @@
       <c r="P110" s="211"/>
       <c r="Q110" s="220"/>
     </row>
-    <row r="111" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="111" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A111" s="152">
         <v>108</v>
       </c>
@@ -10715,7 +10715,7 @@
       <c r="P111" s="211"/>
       <c r="Q111" s="220"/>
     </row>
-    <row r="112" spans="1:17" s="17" customFormat="1" ht="58.5" customHeight="1">
+    <row r="112" spans="1:17" s="17" customFormat="1" ht="58.5" hidden="1" customHeight="1">
       <c r="A112" s="152">
         <v>110</v>
       </c>
@@ -11598,6 +11598,13 @@
     <row r="232" ht="13.8" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A3:Q152">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="熊驰"/>
+        <filter val="熊驰_x000a_周述文"/>
+        <filter val="周述文"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="10">
       <filters>
         <dateGroupItem year="2019" dateTimeGrouping="year"/>

</xml_diff>